<commit_message>
Additions to startupScripts sheet
</commit_message>
<xml_diff>
--- a/StartupScripts/startupScripts.xlsx
+++ b/StartupScripts/startupScripts.xlsx
@@ -11,13 +11,15 @@
     <sheet name="RavenRock" sheetId="2" r:id="rId2"/>
     <sheet name="Strongholds" sheetId="3" r:id="rId3"/>
     <sheet name="Tribuanl Quests" sheetId="4" r:id="rId4"/>
+    <sheet name="Bloodmoon" sheetId="5" r:id="rId5"/>
+    <sheet name="Werewolves" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="306">
   <si>
     <t>;for fallingGuy</t>
   </si>
@@ -472,9 +474,6 @@
     <t>Run the script</t>
   </si>
   <si>
-    <t>&gt; startscript, startup</t>
-  </si>
-  <si>
     <t>&gt; set shrineboethiah.dayspassed to 19</t>
   </si>
   <si>
@@ -694,57 +693,6 @@
     <t>Disable on 100</t>
   </si>
   <si>
-    <t>MournholdAttack = 1</t>
-  </si>
-  <si>
-    <t>forces autogoodbye</t>
-  </si>
-  <si>
-    <t>if ( day != startday )</t>
-  </si>
-  <si>
-    <t>if ( MournholdAttack == 0 )</t>
-  </si>
-  <si>
-    <t>if ( GetPCCell "Mournhold, Plaza Brindisi Dorom" != 1 )</t>
-  </si>
-  <si>
-    <t>set FabAttack to 1</t>
-  </si>
-  <si>
-    <t>set MournholdAttack to 1</t>
-  </si>
-  <si>
-    <t>endif</t>
-  </si>
-  <si>
-    <t>if ( FabAttack == 1 )</t>
-  </si>
-  <si>
-    <t>if ( GetJournalIndex TR_MHAttack &lt; 30 )</t>
-  </si>
-  <si>
-    <t>if ( GetDeadCount "fabricant_hulkin_attack" &gt;= 4 )</t>
-  </si>
-  <si>
-    <t>if ( GetDeadCount "fabricant_verm_attack" &gt;= 4 )</t>
-  </si>
-  <si>
-    <t>journal "tr_mhattack" 30</t>
-  </si>
-  <si>
-    <t>set MournholdAttack to -1</t>
-  </si>
-  <si>
-    <t>set state to -1</t>
-  </si>
-  <si>
-    <t>MHAttack:</t>
-  </si>
-  <si>
-    <t>Solution: Set MournholdAttack to -1 if TR_MHAttack &gt;= 30</t>
-  </si>
-  <si>
     <t>Itermerel</t>
   </si>
   <si>
@@ -923,6 +871,72 @@
   </si>
   <si>
     <t>key_Private_Quarters</t>
+  </si>
+  <si>
+    <t>set werewolfclawmult to 35</t>
+  </si>
+  <si>
+    <t>Start WereChangeScript if PCWerewolf == 1 on login</t>
+  </si>
+  <si>
+    <t>Guards and note thing is currently disregarded</t>
+  </si>
+  <si>
+    <t>Note thing is much less important than the rest</t>
+  </si>
+  <si>
+    <t>Guards need to be replaced by their versions of guard-class NPCs</t>
+  </si>
+  <si>
+    <t>, which I cba to look up atm</t>
+  </si>
+  <si>
+    <t>if bm_ceremony2 == 10</t>
+  </si>
+  <si>
+    <t>dreamcount to 1</t>
+  </si>
+  <si>
+    <t>if bm_bearhunt2 == 10</t>
+  </si>
+  <si>
+    <t>dreamcount to 2</t>
+  </si>
+  <si>
+    <t>if bm_frostgiant2 == 10</t>
+  </si>
+  <si>
+    <t>dreamcount to 3</t>
+  </si>
+  <si>
+    <t>if bm_wildhunt == 25</t>
+  </si>
+  <si>
+    <t>dreamcount to 4</t>
+  </si>
+  <si>
+    <t>if bm_ceremony2 == 100</t>
+  </si>
+  <si>
+    <t>if bm_lycanthropycure == 20</t>
+  </si>
+  <si>
+    <t>set PCWerewolf to -1</t>
+  </si>
+  <si>
+    <t>WereChangeScript variables</t>
+  </si>
+  <si>
+    <t>firstdream to 1</t>
+  </si>
+  <si>
+    <t>if bm_skaalattack == 95</t>
+  </si>
+  <si>
+    <t>set PCWerewolf to 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Set MournholdAttack to -1 if TR_MHAttack &gt;= 30</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1134,6 +1148,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1437,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="H19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,7 +1471,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>1</v>
@@ -1509,7 +1524,7 @@
         <v>50</v>
       </c>
       <c r="K2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M2" t="s">
         <v>11</v>
@@ -1538,7 +1553,7 @@
         <v>100</v>
       </c>
       <c r="K3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M3" t="s">
         <v>19</v>
@@ -1555,7 +1570,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1596,7 +1611,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="10"/>
@@ -1615,10 +1630,10 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>288</v>
+        <v>270</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="10"/>
@@ -1639,11 +1654,11 @@
       <c r="A8" s="11"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="D8" s="10"/>
       <c r="M8" t="s">
-        <v>301</v>
+        <v>283</v>
       </c>
       <c r="N8" t="s">
         <v>25</v>
@@ -1686,7 +1701,7 @@
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
       <c r="F10" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G10" t="s">
         <v>3</v>
@@ -1716,7 +1731,7 @@
         <v>5</v>
       </c>
       <c r="Q10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -1729,7 +1744,7 @@
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
       <c r="G11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H11" t="s">
         <v>38</v>
@@ -1758,15 +1773,15 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="G12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H12" t="s">
         <v>38</v>
@@ -1792,15 +1807,15 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>287</v>
+        <v>269</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>289</v>
+        <v>271</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
       <c r="G13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H13" t="s">
         <v>38</v>
@@ -1826,15 +1841,15 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="16"/>
       <c r="G14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H14" t="s">
         <v>38</v>
@@ -1860,7 +1875,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H15" t="s">
         <v>38</v>
@@ -1889,7 +1904,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H16" t="s">
         <v>38</v>
@@ -1956,7 +1971,7 @@
         <v>61</v>
       </c>
       <c r="K18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M18" t="s">
         <v>137</v>
@@ -1976,7 +1991,7 @@
     </row>
     <row r="19" spans="7:17" x14ac:dyDescent="0.25">
       <c r="K19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M19" t="s">
         <v>138</v>
@@ -1993,7 +2008,7 @@
     </row>
     <row r="20" spans="7:17" x14ac:dyDescent="0.25">
       <c r="K20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M20" t="s">
         <v>144</v>
@@ -2010,7 +2025,7 @@
     </row>
     <row r="21" spans="7:17" x14ac:dyDescent="0.25">
       <c r="K21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M21" t="s">
         <v>145</v>
@@ -2027,16 +2042,16 @@
     </row>
     <row r="22" spans="7:17" x14ac:dyDescent="0.25">
       <c r="K22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N22" t="s">
+        <v>169</v>
+      </c>
+      <c r="O22" t="s">
         <v>170</v>
-      </c>
-      <c r="O22" t="s">
-        <v>171</v>
       </c>
       <c r="P22">
         <v>10</v>
@@ -2044,54 +2059,54 @@
     </row>
     <row r="23" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J23">
         <v>10</v>
       </c>
       <c r="K23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M23" t="s">
+        <v>168</v>
+      </c>
+      <c r="N23" t="s">
         <v>169</v>
       </c>
-      <c r="N23" t="s">
+      <c r="O23" t="s">
         <v>170</v>
       </c>
-      <c r="O23" t="s">
+      <c r="P23">
+        <v>10</v>
+      </c>
+      <c r="Q23" t="s">
         <v>171</v>
-      </c>
-      <c r="P23">
-        <v>10</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="24" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J24">
         <v>10</v>
       </c>
       <c r="M24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="O24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P24">
         <v>10</v>
@@ -2099,22 +2114,22 @@
     </row>
     <row r="25" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J25">
         <v>10</v>
       </c>
       <c r="M25" t="s">
+        <v>181</v>
+      </c>
+      <c r="N25" t="s">
         <v>182</v>
       </c>
-      <c r="N25" t="s">
-        <v>183</v>
-      </c>
       <c r="O25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P25">
         <v>10</v>
@@ -2122,22 +2137,22 @@
     </row>
     <row r="26" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J26">
         <v>10</v>
       </c>
       <c r="M26" t="s">
+        <v>211</v>
+      </c>
+      <c r="N26" t="s">
+        <v>213</v>
+      </c>
+      <c r="O26" t="s">
         <v>212</v>
-      </c>
-      <c r="N26" t="s">
-        <v>214</v>
-      </c>
-      <c r="O26" t="s">
-        <v>213</v>
       </c>
       <c r="P26">
         <v>10</v>
@@ -2145,48 +2160,48 @@
     </row>
     <row r="27" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J27">
         <v>10</v>
       </c>
       <c r="M27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N27" t="s">
+        <v>216</v>
+      </c>
+      <c r="O27" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="O27" s="4" t="s">
+      <c r="P27">
+        <v>10</v>
+      </c>
+      <c r="Q27" t="s">
         <v>218</v>
-      </c>
-      <c r="P27">
-        <v>10</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="28" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J28">
         <v>10</v>
       </c>
       <c r="M28" t="s">
+        <v>215</v>
+      </c>
+      <c r="N28" t="s">
         <v>216</v>
       </c>
-      <c r="N28" t="s">
+      <c r="O28" s="4" t="s">
         <v>217</v>
-      </c>
-      <c r="O28" s="4" t="s">
-        <v>218</v>
       </c>
       <c r="P28">
         <v>10</v>
@@ -2194,109 +2209,109 @@
     </row>
     <row r="29" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J29">
         <v>10</v>
       </c>
       <c r="M29" t="s">
+        <v>220</v>
+      </c>
+      <c r="N29" t="s">
+        <v>220</v>
+      </c>
+      <c r="O29" t="s">
         <v>221</v>
       </c>
-      <c r="N29" t="s">
-        <v>221</v>
-      </c>
-      <c r="O29" t="s">
-        <v>222</v>
-      </c>
       <c r="P29">
         <v>10</v>
       </c>
       <c r="Q29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="30" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J30">
         <v>10</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="O30" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="P30">
+        <v>10</v>
+      </c>
+      <c r="Q30" t="s">
         <v>223</v>
-      </c>
-      <c r="P30">
-        <v>10</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="31" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G31" t="s">
+        <v>164</v>
+      </c>
+      <c r="H31" t="s">
         <v>165</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>166</v>
       </c>
-      <c r="I31" t="s">
-        <v>167</v>
-      </c>
       <c r="J31">
         <v>10</v>
       </c>
       <c r="K31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M31" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="N31" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="O31" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="P31">
         <v>10</v>
       </c>
       <c r="Q31" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H32" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J32">
         <v>10</v>
       </c>
       <c r="M32" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="N32" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="O32" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="P32">
         <v>50</v>
@@ -2304,54 +2319,54 @@
     </row>
     <row r="33" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I33" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J33">
         <v>10</v>
       </c>
       <c r="M33" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="N33" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="O33" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="P33">
         <v>100</v>
       </c>
       <c r="Q33" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
     </row>
     <row r="34" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J34">
         <v>10</v>
       </c>
       <c r="M34" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="N34" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="O34" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="P34">
         <v>10</v>
@@ -2359,25 +2374,25 @@
     </row>
     <row r="35" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G35" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H35" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J35">
         <v>10</v>
       </c>
       <c r="M35" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="N35" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="O35" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="P35">
         <v>10</v>
@@ -2385,123 +2400,123 @@
     </row>
     <row r="36" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G36" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I36" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J36">
         <v>10</v>
       </c>
       <c r="M36" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="N36" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="O36" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="P36">
         <v>10</v>
       </c>
       <c r="Q36" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
+        <v>187</v>
+      </c>
+      <c r="H37" t="s">
         <v>188</v>
       </c>
-      <c r="H37" t="s">
-        <v>189</v>
-      </c>
       <c r="I37" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J37">
         <v>10</v>
       </c>
       <c r="M37" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="N37" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="O37" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
       <c r="P37">
         <v>40</v>
       </c>
       <c r="Q37" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
     </row>
     <row r="38" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G38" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H38" t="s">
+        <v>202</v>
+      </c>
+      <c r="I38" t="s">
         <v>203</v>
-      </c>
-      <c r="I38" t="s">
-        <v>204</v>
       </c>
       <c r="J38">
         <v>50</v>
       </c>
       <c r="M38" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
       <c r="N38" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="O38" t="s">
-        <v>290</v>
+        <v>272</v>
       </c>
       <c r="P38">
         <v>30</v>
       </c>
       <c r="Q38" t="s">
-        <v>293</v>
+        <v>275</v>
       </c>
     </row>
     <row r="39" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G39" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I39" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J39">
         <v>50</v>
       </c>
       <c r="M39" t="s">
-        <v>295</v>
+        <v>277</v>
       </c>
       <c r="N39" t="s">
-        <v>296</v>
+        <v>278</v>
       </c>
       <c r="O39" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
       <c r="P39">
         <v>20</v>
       </c>
       <c r="Q39" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
     </row>
     <row r="40" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G40" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I40" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J40">
         <v>50</v>
@@ -2509,10 +2524,10 @@
     </row>
     <row r="41" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G41" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J41">
         <v>50</v>
@@ -2520,10 +2535,10 @@
     </row>
     <row r="42" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G42" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I42" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J42">
         <v>50</v>
@@ -2531,10 +2546,10 @@
     </row>
     <row r="43" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I43" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J43">
         <v>50</v>
@@ -2542,10 +2557,10 @@
     </row>
     <row r="44" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I44" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J44">
         <v>50</v>
@@ -2553,10 +2568,10 @@
     </row>
     <row r="45" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G45" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I45" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J45">
         <v>50</v>
@@ -2564,10 +2579,10 @@
     </row>
     <row r="46" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G46" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I46" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J46">
         <v>50</v>
@@ -2575,10 +2590,10 @@
     </row>
     <row r="47" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I47" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J47">
         <v>50</v>
@@ -2586,10 +2601,10 @@
     </row>
     <row r="48" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G48" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I48" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J48">
         <v>50</v>
@@ -2597,10 +2612,10 @@
     </row>
     <row r="49" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G49" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I49" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J49">
         <v>50</v>
@@ -2608,10 +2623,10 @@
     </row>
     <row r="50" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G50" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I50" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J50">
         <v>50</v>
@@ -2627,8 +2642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2863,6 +2878,9 @@
       <c r="F11" s="14" t="s">
         <v>103</v>
       </c>
+      <c r="H11" s="26" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
@@ -2883,6 +2901,9 @@
       <c r="F12" s="10" t="s">
         <v>108</v>
       </c>
+      <c r="H12" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
@@ -2903,6 +2924,9 @@
       <c r="F13" s="10" t="s">
         <v>113</v>
       </c>
+      <c r="H13" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
@@ -2922,6 +2946,9 @@
       </c>
       <c r="F14" s="16" t="s">
         <v>118</v>
+      </c>
+      <c r="H14" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -3067,104 +3094,104 @@
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
       <c r="E1" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
       <c r="H1" t="s">
-        <v>285</v>
+        <v>267</v>
       </c>
       <c r="I1" t="s">
-        <v>277</v>
+        <v>259</v>
       </c>
       <c r="L1" t="s">
-        <v>286</v>
+        <v>268</v>
       </c>
       <c r="M1" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="E2" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="I2" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="M2" t="s">
-        <v>282</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="E4" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="H4" t="s">
-        <v>285</v>
+        <v>267</v>
       </c>
       <c r="I4" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
       <c r="L4" t="s">
-        <v>286</v>
+        <v>268</v>
       </c>
       <c r="M4" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="E5" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="I5" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="M5" t="s">
-        <v>282</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="E7" t="s">
-        <v>276</v>
+        <v>258</v>
       </c>
       <c r="H7" t="s">
-        <v>285</v>
+        <v>267</v>
       </c>
       <c r="I7" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="L7" t="s">
-        <v>286</v>
+        <v>268</v>
       </c>
       <c r="M7" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="E8" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="I8" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="M8" t="s">
-        <v>282</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -3174,128 +3201,122 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:G28"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>225</v>
-      </c>
-      <c r="D7" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F10" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G11" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G12" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F20" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F21" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F22" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E23" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>241</v>
-      </c>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>301</v>
+      </c>
+      <c r="D1" t="s">
+        <v>290</v>
+      </c>
+      <c r="G1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>291</v>
+      </c>
+      <c r="G2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>303</v>
+      </c>
+      <c r="D3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>304</v>
+      </c>
+      <c r="D4" t="s">
+        <v>292</v>
+      </c>
+      <c r="G4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>293</v>
+      </c>
+      <c r="G5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>285</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update literally everything (except CQs)
</commit_message>
<xml_diff>
--- a/StartupScripts/startupScripts.xlsx
+++ b/StartupScripts/startupScripts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="315">
   <si>
     <t>;for fallingGuy</t>
   </si>
@@ -576,9 +576,6 @@
     <t>Same as b4</t>
   </si>
   <si>
-    <t>Dont need to do anything</t>
-  </si>
-  <si>
     <t>DA_Sheogorath</t>
   </si>
   <si>
@@ -937,6 +934,36 @@
   </si>
   <si>
     <t xml:space="preserve"> Set MournholdAttack to -1 if TR_MHAttack &gt;= 30</t>
+  </si>
+  <si>
+    <t>Dont need to do anything to reenable</t>
+  </si>
+  <si>
+    <t>disable on 45</t>
+  </si>
+  <si>
+    <t>disable on IC30_Imperial_veteran 1</t>
+  </si>
+  <si>
+    <t>Disable on 60/110 ms_hannat</t>
+  </si>
+  <si>
+    <t>dont need to disable either of them</t>
+  </si>
+  <si>
+    <t>disable on 70/200</t>
+  </si>
+  <si>
+    <t>disable on 70</t>
+  </si>
+  <si>
+    <t>disable on 75/110</t>
+  </si>
+  <si>
+    <t>disable on 70/110</t>
+  </si>
+  <si>
+    <t>disable on 50/55</t>
   </si>
 </sst>
 </file>
@@ -1452,8 +1479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="J16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1471,7 +1498,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>1</v>
@@ -1524,7 +1551,7 @@
         <v>50</v>
       </c>
       <c r="K2" t="s">
-        <v>185</v>
+        <v>305</v>
       </c>
       <c r="M2" t="s">
         <v>11</v>
@@ -1553,7 +1580,7 @@
         <v>100</v>
       </c>
       <c r="K3" t="s">
-        <v>185</v>
+        <v>305</v>
       </c>
       <c r="M3" t="s">
         <v>19</v>
@@ -1570,7 +1597,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1586,6 +1613,9 @@
       </c>
       <c r="P4">
         <v>10</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -1611,7 +1641,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="10"/>
@@ -1630,10 +1660,10 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="10"/>
@@ -1649,16 +1679,19 @@
       <c r="P7">
         <v>50</v>
       </c>
+      <c r="Q7" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D8" s="10"/>
       <c r="M8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="N8" t="s">
         <v>25</v>
@@ -1690,6 +1723,9 @@
       <c r="P9">
         <v>50</v>
       </c>
+      <c r="Q9" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
@@ -1701,7 +1737,7 @@
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
       <c r="F10" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G10" t="s">
         <v>3</v>
@@ -1731,7 +1767,7 @@
         <v>5</v>
       </c>
       <c r="Q10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -1744,7 +1780,7 @@
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
       <c r="G11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H11" t="s">
         <v>38</v>
@@ -1770,18 +1806,21 @@
       <c r="P11">
         <v>40</v>
       </c>
+      <c r="Q11" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>237</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>238</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="G12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H12" t="s">
         <v>38</v>
@@ -1807,15 +1846,15 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
       <c r="G13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H13" t="s">
         <v>38</v>
@@ -1838,18 +1877,21 @@
       <c r="P13">
         <v>10</v>
       </c>
+      <c r="Q13" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
+        <v>279</v>
+      </c>
+      <c r="B14" s="25" t="s">
         <v>280</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>281</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="16"/>
       <c r="G14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H14" t="s">
         <v>38</v>
@@ -1875,7 +1917,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H15" t="s">
         <v>38</v>
@@ -1904,7 +1946,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H16" t="s">
         <v>38</v>
@@ -2005,6 +2047,9 @@
       <c r="P19" t="s">
         <v>140</v>
       </c>
+      <c r="Q19" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="20" spans="7:17" x14ac:dyDescent="0.25">
       <c r="K20" t="s">
@@ -2022,6 +2067,9 @@
       <c r="P20">
         <v>10</v>
       </c>
+      <c r="Q20" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="21" spans="7:17" x14ac:dyDescent="0.25">
       <c r="K21" t="s">
@@ -2039,6 +2087,9 @@
       <c r="P21">
         <v>10</v>
       </c>
+      <c r="Q21" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="22" spans="7:17" x14ac:dyDescent="0.25">
       <c r="K22" t="s">
@@ -2056,6 +2107,9 @@
       <c r="P22">
         <v>10</v>
       </c>
+      <c r="Q22" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="23" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G23" t="s">
@@ -2146,13 +2200,13 @@
         <v>10</v>
       </c>
       <c r="M26" t="s">
+        <v>210</v>
+      </c>
+      <c r="N26" t="s">
+        <v>212</v>
+      </c>
+      <c r="O26" t="s">
         <v>211</v>
-      </c>
-      <c r="N26" t="s">
-        <v>213</v>
-      </c>
-      <c r="O26" t="s">
-        <v>212</v>
       </c>
       <c r="P26">
         <v>10</v>
@@ -2169,19 +2223,19 @@
         <v>10</v>
       </c>
       <c r="M27" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N27" t="s">
+        <v>215</v>
+      </c>
+      <c r="O27" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="O27" s="4" t="s">
+      <c r="P27">
+        <v>10</v>
+      </c>
+      <c r="Q27" t="s">
         <v>217</v>
-      </c>
-      <c r="P27">
-        <v>10</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="28" spans="7:17" x14ac:dyDescent="0.25">
@@ -2195,13 +2249,13 @@
         <v>10</v>
       </c>
       <c r="M28" t="s">
+        <v>214</v>
+      </c>
+      <c r="N28" t="s">
         <v>215</v>
       </c>
-      <c r="N28" t="s">
+      <c r="O28" s="4" t="s">
         <v>216</v>
-      </c>
-      <c r="O28" s="4" t="s">
-        <v>217</v>
       </c>
       <c r="P28">
         <v>10</v>
@@ -2218,19 +2272,19 @@
         <v>10</v>
       </c>
       <c r="M29" t="s">
+        <v>219</v>
+      </c>
+      <c r="N29" t="s">
+        <v>219</v>
+      </c>
+      <c r="O29" t="s">
         <v>220</v>
       </c>
-      <c r="N29" t="s">
-        <v>220</v>
-      </c>
-      <c r="O29" t="s">
-        <v>221</v>
-      </c>
       <c r="P29">
         <v>10</v>
       </c>
       <c r="Q29" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="30" spans="7:17" x14ac:dyDescent="0.25">
@@ -2244,19 +2298,19 @@
         <v>10</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O30" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="P30">
+        <v>10</v>
+      </c>
+      <c r="Q30" t="s">
         <v>222</v>
-      </c>
-      <c r="P30">
-        <v>10</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="31" spans="7:17" x14ac:dyDescent="0.25">
@@ -2276,19 +2330,19 @@
         <v>184</v>
       </c>
       <c r="M31" t="s">
+        <v>224</v>
+      </c>
+      <c r="N31" t="s">
+        <v>224</v>
+      </c>
+      <c r="O31" t="s">
         <v>225</v>
       </c>
-      <c r="N31" t="s">
-        <v>225</v>
-      </c>
-      <c r="O31" t="s">
-        <v>226</v>
-      </c>
       <c r="P31">
         <v>10</v>
       </c>
       <c r="Q31" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="32" spans="7:17" x14ac:dyDescent="0.25">
@@ -2305,13 +2359,13 @@
         <v>10</v>
       </c>
       <c r="M32" t="s">
+        <v>227</v>
+      </c>
+      <c r="N32" t="s">
         <v>228</v>
       </c>
-      <c r="N32" t="s">
-        <v>229</v>
-      </c>
       <c r="O32" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="P32">
         <v>50</v>
@@ -2331,19 +2385,19 @@
         <v>10</v>
       </c>
       <c r="M33" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="O33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="P33">
         <v>100</v>
       </c>
       <c r="Q33" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="34" spans="7:17" x14ac:dyDescent="0.25">
@@ -2360,16 +2414,19 @@
         <v>10</v>
       </c>
       <c r="M34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="N34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P34">
         <v>10</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="35" spans="7:17" x14ac:dyDescent="0.25">
@@ -2386,13 +2443,13 @@
         <v>10</v>
       </c>
       <c r="M35" t="s">
+        <v>233</v>
+      </c>
+      <c r="N35" t="s">
         <v>234</v>
       </c>
-      <c r="N35" t="s">
+      <c r="O35" t="s">
         <v>235</v>
-      </c>
-      <c r="O35" t="s">
-        <v>236</v>
       </c>
       <c r="P35">
         <v>10</v>
@@ -2412,111 +2469,111 @@
         <v>10</v>
       </c>
       <c r="M36" t="s">
+        <v>239</v>
+      </c>
+      <c r="N36" t="s">
         <v>240</v>
       </c>
-      <c r="N36" t="s">
+      <c r="O36" t="s">
+        <v>238</v>
+      </c>
+      <c r="P36">
+        <v>10</v>
+      </c>
+      <c r="Q36" t="s">
         <v>241</v>
-      </c>
-      <c r="O36" t="s">
-        <v>239</v>
-      </c>
-      <c r="P36">
-        <v>10</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="37" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
+        <v>186</v>
+      </c>
+      <c r="H37" t="s">
         <v>187</v>
       </c>
-      <c r="H37" t="s">
-        <v>188</v>
-      </c>
       <c r="I37" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J37">
         <v>10</v>
       </c>
       <c r="M37" t="s">
+        <v>245</v>
+      </c>
+      <c r="N37" t="s">
+        <v>247</v>
+      </c>
+      <c r="O37" t="s">
         <v>246</v>
-      </c>
-      <c r="N37" t="s">
-        <v>248</v>
-      </c>
-      <c r="O37" t="s">
-        <v>247</v>
       </c>
       <c r="P37">
         <v>40</v>
       </c>
       <c r="Q37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="38" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G38" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H38" t="s">
+        <v>201</v>
+      </c>
+      <c r="I38" t="s">
         <v>202</v>
-      </c>
-      <c r="I38" t="s">
-        <v>203</v>
       </c>
       <c r="J38">
         <v>50</v>
       </c>
       <c r="M38" t="s">
+        <v>272</v>
+      </c>
+      <c r="N38" t="s">
         <v>273</v>
       </c>
-      <c r="N38" t="s">
-        <v>274</v>
-      </c>
       <c r="O38" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="P38">
         <v>30</v>
       </c>
       <c r="Q38" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="39" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G39" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I39" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J39">
         <v>50</v>
       </c>
       <c r="M39" t="s">
+        <v>276</v>
+      </c>
+      <c r="N39" t="s">
         <v>277</v>
       </c>
-      <c r="N39" t="s">
-        <v>278</v>
-      </c>
       <c r="O39" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="P39">
         <v>20</v>
       </c>
       <c r="Q39" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="40" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G40" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I40" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J40">
         <v>50</v>
@@ -2524,10 +2581,10 @@
     </row>
     <row r="41" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I41" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J41">
         <v>50</v>
@@ -2535,10 +2592,10 @@
     </row>
     <row r="42" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G42" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J42">
         <v>50</v>
@@ -2546,10 +2603,10 @@
     </row>
     <row r="43" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I43" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J43">
         <v>50</v>
@@ -2557,10 +2614,10 @@
     </row>
     <row r="44" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I44" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J44">
         <v>50</v>
@@ -2568,10 +2625,10 @@
     </row>
     <row r="45" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G45" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I45" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J45">
         <v>50</v>
@@ -2579,10 +2636,10 @@
     </row>
     <row r="46" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G46" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I46" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J46">
         <v>50</v>
@@ -2590,10 +2647,10 @@
     </row>
     <row r="47" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I47" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J47">
         <v>50</v>
@@ -2601,10 +2658,10 @@
     </row>
     <row r="48" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G48" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I48" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J48">
         <v>50</v>
@@ -2612,10 +2669,10 @@
     </row>
     <row r="49" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G49" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I49" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J49">
         <v>50</v>
@@ -2623,10 +2680,10 @@
     </row>
     <row r="50" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G50" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I50" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J50">
         <v>50</v>
@@ -2642,8 +2699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2666,7 +2723,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>61</v>
@@ -2879,7 +2936,7 @@
         <v>103</v>
       </c>
       <c r="H11" s="26" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2902,7 +2959,7 @@
         <v>108</v>
       </c>
       <c r="H12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -2925,7 +2982,7 @@
         <v>113</v>
       </c>
       <c r="H13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2948,7 +3005,7 @@
         <v>118</v>
       </c>
       <c r="H14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -3094,104 +3151,104 @@
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H1" t="s">
+        <v>266</v>
+      </c>
+      <c r="I1" t="s">
+        <v>258</v>
+      </c>
+      <c r="L1" t="s">
         <v>267</v>
       </c>
-      <c r="I1" t="s">
-        <v>259</v>
-      </c>
-      <c r="L1" t="s">
-        <v>268</v>
-      </c>
       <c r="M1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H4" t="s">
+        <v>266</v>
+      </c>
+      <c r="I4" t="s">
+        <v>260</v>
+      </c>
+      <c r="L4" t="s">
         <v>267</v>
       </c>
-      <c r="I4" t="s">
-        <v>261</v>
-      </c>
-      <c r="L4" t="s">
-        <v>268</v>
-      </c>
       <c r="M4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H7" t="s">
+        <v>266</v>
+      </c>
+      <c r="I7" t="s">
+        <v>261</v>
+      </c>
+      <c r="L7" t="s">
         <v>267</v>
       </c>
-      <c r="I7" t="s">
-        <v>262</v>
-      </c>
-      <c r="L7" t="s">
-        <v>268</v>
-      </c>
       <c r="M7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -3211,7 +3268,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3239,80 +3296,80 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the script for 0.7.0
</commit_message>
<xml_diff>
--- a/StartupScripts/startupScripts.xlsx
+++ b/StartupScripts/startupScripts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="347">
   <si>
     <t>;for fallingGuy</t>
   </si>
@@ -964,6 +964,102 @@
   </si>
   <si>
     <t>disable on 50/55</t>
+  </si>
+  <si>
+    <t>Stones:</t>
+  </si>
+  <si>
+    <t>Quest ID</t>
+  </si>
+  <si>
+    <t>Completion index</t>
+  </si>
+  <si>
+    <t>Beast</t>
+  </si>
+  <si>
+    <t>BM_Beasts</t>
+  </si>
+  <si>
+    <t>BM_Stones index</t>
+  </si>
+  <si>
+    <t>Done index</t>
+  </si>
+  <si>
+    <t>Earth</t>
+  </si>
+  <si>
+    <t>Particles</t>
+  </si>
+  <si>
+    <t>Act_BM_Beast_parts</t>
+  </si>
+  <si>
+    <t>BM_Earth</t>
+  </si>
+  <si>
+    <t>Act_BM_Earth_parts</t>
+  </si>
+  <si>
+    <t>Sun</t>
+  </si>
+  <si>
+    <t>Trees</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>Act_BM_Sun_parts</t>
+  </si>
+  <si>
+    <t>BM_Sun</t>
+  </si>
+  <si>
+    <t>Act_BM_Tree_parts</t>
+  </si>
+  <si>
+    <t>BM_Trees</t>
+  </si>
+  <si>
+    <t>Act_BM_Water_parts</t>
+  </si>
+  <si>
+    <t>BM_Water</t>
+  </si>
+  <si>
+    <t>BM_Wind</t>
+  </si>
+  <si>
+    <t>Act_BM_Wind_parts</t>
+  </si>
+  <si>
+    <t>for each stone, set stones to ( stones ) +1</t>
+  </si>
+  <si>
+    <t>additionally, set doOnce to 1 on stones if quest index &gt; 10, 2 if quest index = 100</t>
+  </si>
+  <si>
+    <t>Act_BM_stone_&lt;thing&gt;_01</t>
+  </si>
+  <si>
+    <t>Karrod:</t>
+  </si>
+  <si>
+    <t>if TR_Champion == 20, set KarrodFightStart to 1, start karrodMovement script</t>
+  </si>
+  <si>
+    <t>if TR_Champion == 50, set KarrodBribe to 1</t>
+  </si>
+  <si>
+    <t>TR_Blade == 60 then start bladefixScript</t>
+  </si>
+  <si>
+    <t>Start BMStartUpScript on empty server</t>
   </si>
 </sst>
 </file>
@@ -1479,8 +1575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView topLeftCell="J16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3258,10 +3354,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3271,8 +3367,26 @@
         <v>304</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>343</v>
+      </c>
+    </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>344</v>
+      </c>
       <c r="B5" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>345</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3281,12 +3395,179 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="7" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D2" t="s">
+        <v>317</v>
+      </c>
+      <c r="E2" t="s">
+        <v>321</v>
+      </c>
+      <c r="F2" t="s">
+        <v>320</v>
+      </c>
+      <c r="G2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C3" t="s">
+        <v>319</v>
+      </c>
+      <c r="D3">
+        <v>50</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3">
+        <v>66</v>
+      </c>
+      <c r="G3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>322</v>
+      </c>
+      <c r="C4" t="s">
+        <v>325</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
+      <c r="F4">
+        <v>62</v>
+      </c>
+      <c r="G4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>327</v>
+      </c>
+      <c r="C5" t="s">
+        <v>332</v>
+      </c>
+      <c r="D5">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <v>68</v>
+      </c>
+      <c r="G5" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>328</v>
+      </c>
+      <c r="C6" t="s">
+        <v>334</v>
+      </c>
+      <c r="D6">
+        <v>40</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>64</v>
+      </c>
+      <c r="G6" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>329</v>
+      </c>
+      <c r="C7" t="s">
+        <v>336</v>
+      </c>
+      <c r="D7">
+        <v>70</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>60</v>
+      </c>
+      <c r="G7" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>330</v>
+      </c>
+      <c r="C8" t="s">
+        <v>337</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>70</v>
+      </c>
+      <c r="G8" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>346</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>